<commit_message>
bug uploade Teilnehmer liste fixed
</commit_message>
<xml_diff>
--- a/files/Teilnehmer.xlsx
+++ b/files/Teilnehmer.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell Latitude\PycharmProjects\dlrg_wettkampf\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feuer\PycharmProjects\dlrg_wettkampf\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB09965D-6115-4A24-A7E0-96464C6CA94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="8770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2625" yWindow="2625" windowWidth="14400" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="202">
   <si>
     <t>Vorname</t>
   </si>
@@ -118,24 +117,6 @@
     <t>AK2</t>
   </si>
   <si>
-    <t>AK3</t>
-  </si>
-  <si>
-    <t>AK4</t>
-  </si>
-  <si>
-    <t>AK5</t>
-  </si>
-  <si>
-    <t>AK6</t>
-  </si>
-  <si>
-    <t>AK7</t>
-  </si>
-  <si>
-    <t>AK8</t>
-  </si>
-  <si>
     <t>Teilnehmer Nummer</t>
   </si>
   <si>
@@ -184,25 +165,472 @@
     <t>DLRG LDS 13</t>
   </si>
   <si>
-    <t>AK9</t>
-  </si>
-  <si>
-    <t>AK10</t>
-  </si>
-  <si>
-    <t>AK11</t>
-  </si>
-  <si>
-    <t>AK12</t>
-  </si>
-  <si>
-    <t>AK13</t>
+    <t>DLRG LDS 14</t>
+  </si>
+  <si>
+    <t>DLRG LDS 15</t>
+  </si>
+  <si>
+    <t>DLRG LDS 16</t>
+  </si>
+  <si>
+    <t>DLRG LDS 17</t>
+  </si>
+  <si>
+    <t>DLRG LDS 18</t>
+  </si>
+  <si>
+    <t>DLRG LDS 19</t>
+  </si>
+  <si>
+    <t>DLRG LDS 20</t>
+  </si>
+  <si>
+    <t>DLRG LDS 21</t>
+  </si>
+  <si>
+    <t>DLRG LDS 22</t>
+  </si>
+  <si>
+    <t>DLRG LDS 23</t>
+  </si>
+  <si>
+    <t>DLRG LDS 24</t>
+  </si>
+  <si>
+    <t>DLRG LDS 25</t>
+  </si>
+  <si>
+    <t>DLRG LDS 26</t>
+  </si>
+  <si>
+    <t>DLRG LDS 27</t>
+  </si>
+  <si>
+    <t>Walther14</t>
+  </si>
+  <si>
+    <t>Walther15</t>
+  </si>
+  <si>
+    <t>Walther16</t>
+  </si>
+  <si>
+    <t>Walther17</t>
+  </si>
+  <si>
+    <t>Walther18</t>
+  </si>
+  <si>
+    <t>Walther19</t>
+  </si>
+  <si>
+    <t>Walther20</t>
+  </si>
+  <si>
+    <t>Walther21</t>
+  </si>
+  <si>
+    <t>Walther22</t>
+  </si>
+  <si>
+    <t>Walther23</t>
+  </si>
+  <si>
+    <t>Walther24</t>
+  </si>
+  <si>
+    <t>Walther25</t>
+  </si>
+  <si>
+    <t>Walther26</t>
+  </si>
+  <si>
+    <t>Walther27</t>
+  </si>
+  <si>
+    <t>Emil14</t>
+  </si>
+  <si>
+    <t>Emil15</t>
+  </si>
+  <si>
+    <t>Emil16</t>
+  </si>
+  <si>
+    <t>Emil17</t>
+  </si>
+  <si>
+    <t>Emil18</t>
+  </si>
+  <si>
+    <t>Emil19</t>
+  </si>
+  <si>
+    <t>Emil20</t>
+  </si>
+  <si>
+    <t>Emil21</t>
+  </si>
+  <si>
+    <t>Emil22</t>
+  </si>
+  <si>
+    <t>Emil23</t>
+  </si>
+  <si>
+    <t>Emil24</t>
+  </si>
+  <si>
+    <t>Emil25</t>
+  </si>
+  <si>
+    <t>Emil26</t>
+  </si>
+  <si>
+    <t>Emil27</t>
+  </si>
+  <si>
+    <t>Emil28</t>
+  </si>
+  <si>
+    <t>Emil29</t>
+  </si>
+  <si>
+    <t>Emil30</t>
+  </si>
+  <si>
+    <t>Emil31</t>
+  </si>
+  <si>
+    <t>Emil32</t>
+  </si>
+  <si>
+    <t>Emil33</t>
+  </si>
+  <si>
+    <t>Emil34</t>
+  </si>
+  <si>
+    <t>Emil35</t>
+  </si>
+  <si>
+    <t>Emil36</t>
+  </si>
+  <si>
+    <t>Emil37</t>
+  </si>
+  <si>
+    <t>Emil38</t>
+  </si>
+  <si>
+    <t>Emil39</t>
+  </si>
+  <si>
+    <t>Emil40</t>
+  </si>
+  <si>
+    <t>Emil41</t>
+  </si>
+  <si>
+    <t>Emil42</t>
+  </si>
+  <si>
+    <t>Emil43</t>
+  </si>
+  <si>
+    <t>Emil44</t>
+  </si>
+  <si>
+    <t>Emil45</t>
+  </si>
+  <si>
+    <t>Emil46</t>
+  </si>
+  <si>
+    <t>Emil47</t>
+  </si>
+  <si>
+    <t>Emil48</t>
+  </si>
+  <si>
+    <t>Emil49</t>
+  </si>
+  <si>
+    <t>Emil50</t>
+  </si>
+  <si>
+    <t>Emil51</t>
+  </si>
+  <si>
+    <t>Emil52</t>
+  </si>
+  <si>
+    <t>Emil53</t>
+  </si>
+  <si>
+    <t>Emil54</t>
+  </si>
+  <si>
+    <t>Emil55</t>
+  </si>
+  <si>
+    <t>Emil56</t>
+  </si>
+  <si>
+    <t>Emil57</t>
+  </si>
+  <si>
+    <t>Emil58</t>
+  </si>
+  <si>
+    <t>Emil59</t>
+  </si>
+  <si>
+    <t>Emil60</t>
+  </si>
+  <si>
+    <t>Emil61</t>
+  </si>
+  <si>
+    <t>Emil62</t>
+  </si>
+  <si>
+    <t>Emil63</t>
+  </si>
+  <si>
+    <t>Emil64</t>
+  </si>
+  <si>
+    <t>Walther28</t>
+  </si>
+  <si>
+    <t>Walther29</t>
+  </si>
+  <si>
+    <t>Walther30</t>
+  </si>
+  <si>
+    <t>Walther31</t>
+  </si>
+  <si>
+    <t>Walther32</t>
+  </si>
+  <si>
+    <t>Walther33</t>
+  </si>
+  <si>
+    <t>Walther34</t>
+  </si>
+  <si>
+    <t>Walther35</t>
+  </si>
+  <si>
+    <t>Walther36</t>
+  </si>
+  <si>
+    <t>Walther37</t>
+  </si>
+  <si>
+    <t>Walther38</t>
+  </si>
+  <si>
+    <t>Walther39</t>
+  </si>
+  <si>
+    <t>Walther40</t>
+  </si>
+  <si>
+    <t>Walther41</t>
+  </si>
+  <si>
+    <t>Walther42</t>
+  </si>
+  <si>
+    <t>Walther43</t>
+  </si>
+  <si>
+    <t>Walther44</t>
+  </si>
+  <si>
+    <t>Walther45</t>
+  </si>
+  <si>
+    <t>Walther46</t>
+  </si>
+  <si>
+    <t>Walther47</t>
+  </si>
+  <si>
+    <t>Walther48</t>
+  </si>
+  <si>
+    <t>Walther49</t>
+  </si>
+  <si>
+    <t>Walther50</t>
+  </si>
+  <si>
+    <t>Walther51</t>
+  </si>
+  <si>
+    <t>Walther52</t>
+  </si>
+  <si>
+    <t>Walther53</t>
+  </si>
+  <si>
+    <t>Walther54</t>
+  </si>
+  <si>
+    <t>Walther55</t>
+  </si>
+  <si>
+    <t>Walther56</t>
+  </si>
+  <si>
+    <t>Walther57</t>
+  </si>
+  <si>
+    <t>Walther58</t>
+  </si>
+  <si>
+    <t>Walther59</t>
+  </si>
+  <si>
+    <t>Walther60</t>
+  </si>
+  <si>
+    <t>Walther61</t>
+  </si>
+  <si>
+    <t>Walther62</t>
+  </si>
+  <si>
+    <t>Walther63</t>
+  </si>
+  <si>
+    <t>Walther64</t>
+  </si>
+  <si>
+    <t>DLRG LDS 28</t>
+  </si>
+  <si>
+    <t>DLRG LDS 29</t>
+  </si>
+  <si>
+    <t>DLRG LDS 30</t>
+  </si>
+  <si>
+    <t>DLRG LDS 31</t>
+  </si>
+  <si>
+    <t>DLRG LDS 32</t>
+  </si>
+  <si>
+    <t>DLRG LDS 33</t>
+  </si>
+  <si>
+    <t>DLRG LDS 34</t>
+  </si>
+  <si>
+    <t>DLRG LDS 35</t>
+  </si>
+  <si>
+    <t>DLRG LDS 36</t>
+  </si>
+  <si>
+    <t>DLRG LDS 37</t>
+  </si>
+  <si>
+    <t>DLRG LDS 38</t>
+  </si>
+  <si>
+    <t>DLRG LDS 39</t>
+  </si>
+  <si>
+    <t>DLRG LDS 40</t>
+  </si>
+  <si>
+    <t>DLRG LDS 41</t>
+  </si>
+  <si>
+    <t>DLRG LDS 42</t>
+  </si>
+  <si>
+    <t>DLRG LDS 43</t>
+  </si>
+  <si>
+    <t>DLRG LDS 44</t>
+  </si>
+  <si>
+    <t>DLRG LDS 45</t>
+  </si>
+  <si>
+    <t>DLRG LDS 46</t>
+  </si>
+  <si>
+    <t>DLRG LDS 47</t>
+  </si>
+  <si>
+    <t>DLRG LDS 48</t>
+  </si>
+  <si>
+    <t>DLRG LDS 49</t>
+  </si>
+  <si>
+    <t>DLRG LDS 50</t>
+  </si>
+  <si>
+    <t>DLRG LDS 51</t>
+  </si>
+  <si>
+    <t>DLRG LDS 52</t>
+  </si>
+  <si>
+    <t>DLRG LDS 53</t>
+  </si>
+  <si>
+    <t>DLRG LDS 54</t>
+  </si>
+  <si>
+    <t>DLRG LDS 55</t>
+  </si>
+  <si>
+    <t>DLRG LDS 56</t>
+  </si>
+  <si>
+    <t>DLRG LDS 57</t>
+  </si>
+  <si>
+    <t>DLRG LDS 58</t>
+  </si>
+  <si>
+    <t>DLRG LDS 59</t>
+  </si>
+  <si>
+    <t>DLRG LDS 60</t>
+  </si>
+  <si>
+    <t>DLRG LDS 61</t>
+  </si>
+  <si>
+    <t>DLRG LDS 62</t>
+  </si>
+  <si>
+    <t>DLRG LDS 63</t>
+  </si>
+  <si>
+    <t>DLRG LDS 64</t>
+  </si>
+  <si>
+    <t>2200m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -265,7 +693,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,21 +992,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -596,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -613,10 +1043,10 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -630,13 +1060,13 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -650,13 +1080,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -670,13 +1100,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -690,13 +1120,13 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -710,13 +1140,13 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -730,13 +1160,13 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -750,109 +1180,1129 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>186</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" t="s">
+        <v>193</v>
+      </c>
+      <c r="E58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>58</v>
       </c>
-      <c r="F14" t="s">
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
+        <v>194</v>
+      </c>
+      <c r="E59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" t="s">
+        <v>195</v>
+      </c>
+      <c r="E60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>159</v>
+      </c>
+      <c r="D61" t="s">
+        <v>196</v>
+      </c>
+      <c r="E61" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D63" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>163</v>
+      </c>
+      <c r="D65" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
teilnehmer bekommen pro disziplin eine Startnummer
</commit_message>
<xml_diff>
--- a/files/Teilnehmer.xlsx
+++ b/files/Teilnehmer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell Latitude\Documents\nextcloud\documente\DLRG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B45B6C9-A43A-40ED-A9CD-367503A34C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692306E8-79B2-4C65-8C66-FE16C45AB5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{1B911A9F-2B35-4147-9F9A-FF8A28EC43AB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$3:$M$201</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="291">
   <si>
     <t>Name</t>
   </si>
@@ -641,7 +641,277 @@
     <t>Stand 12.06.2023</t>
   </si>
   <si>
-    <t>Teilnehmer Nummer</t>
+    <t>Stoilkov</t>
+  </si>
+  <si>
+    <t>Andre´</t>
+  </si>
+  <si>
+    <t>andre.stoilkov@web.de</t>
+  </si>
+  <si>
+    <t>Anika</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Riech</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Humbolt-Gymnasium Eichwalde</t>
+  </si>
+  <si>
+    <t>lisariech7@gmail.com</t>
+  </si>
+  <si>
+    <t>Otto</t>
+  </si>
+  <si>
+    <t>SSV PCK 90 Schwedt e.V.</t>
+  </si>
+  <si>
+    <t>info@ncomputer.de</t>
+  </si>
+  <si>
+    <t>Sasse</t>
+  </si>
+  <si>
+    <t>Cedric</t>
+  </si>
+  <si>
+    <t>Krämer</t>
+  </si>
+  <si>
+    <t>Sven</t>
+  </si>
+  <si>
+    <t>Bowitz</t>
+  </si>
+  <si>
+    <t>Lilien</t>
+  </si>
+  <si>
+    <t>Rotsch</t>
+  </si>
+  <si>
+    <t>Frederike</t>
+  </si>
+  <si>
+    <t>Sobieray</t>
+  </si>
+  <si>
+    <t>Elina</t>
+  </si>
+  <si>
+    <t>annett-sobieray@t-online.de</t>
+  </si>
+  <si>
+    <t>Grundschule Friedersdorf</t>
+  </si>
+  <si>
+    <t>Wachtel</t>
+  </si>
+  <si>
+    <t>Antje.Wachtel@outlook.de</t>
+  </si>
+  <si>
+    <t>Meischeider</t>
+  </si>
+  <si>
+    <t>Amelie</t>
+  </si>
+  <si>
+    <t>anne.meischeider@gmail.com</t>
+  </si>
+  <si>
+    <t>Schultz</t>
+  </si>
+  <si>
+    <t>Bernd</t>
+  </si>
+  <si>
+    <t>HSV Medizin Magdeburg</t>
+  </si>
+  <si>
+    <t>bs@hoppe-und-schultz.de</t>
+  </si>
+  <si>
+    <t>Kelling</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>andreas.Kelling@arcor.de</t>
+  </si>
+  <si>
+    <t>Schröder</t>
+  </si>
+  <si>
+    <t>Guido</t>
+  </si>
+  <si>
+    <t>guido_berlin@web.de</t>
+  </si>
+  <si>
+    <t>Leni</t>
+  </si>
+  <si>
+    <t>Bernsee</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>BSG Pneutmant Wasserball</t>
+  </si>
+  <si>
+    <t>m.bernsee3009@gmail.com</t>
+  </si>
+  <si>
+    <t>Nitschke</t>
+  </si>
+  <si>
+    <t>antje-nitschke@gmx.de</t>
+  </si>
+  <si>
+    <t>Westphal</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>SV Berolina</t>
+  </si>
+  <si>
+    <t>chwestphal@freenet.de</t>
+  </si>
+  <si>
+    <t>Klossek</t>
+  </si>
+  <si>
+    <t>Luke Jared</t>
+  </si>
+  <si>
+    <t>Stand 15.06.2023</t>
+  </si>
+  <si>
+    <t>Drexler</t>
+  </si>
+  <si>
+    <t>Ralf</t>
+  </si>
+  <si>
+    <t>ralf-drexler@web.de</t>
+  </si>
+  <si>
+    <t>Sieke</t>
+  </si>
+  <si>
+    <t>Reinhard</t>
+  </si>
+  <si>
+    <t>Chantal</t>
+  </si>
+  <si>
+    <t>Niemeier</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Rode</t>
+  </si>
+  <si>
+    <t>Mariella</t>
+  </si>
+  <si>
+    <t>Streck</t>
+  </si>
+  <si>
+    <t>Miriam</t>
+  </si>
+  <si>
+    <t>Silvina</t>
+  </si>
+  <si>
+    <t>Pose</t>
+  </si>
+  <si>
+    <t>Thimm</t>
+  </si>
+  <si>
+    <t>Josefine</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Gunnar</t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>Wissing</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Marco10.5@web.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan </t>
+  </si>
+  <si>
+    <t>janrose33@aol.com</t>
+  </si>
+  <si>
+    <t>Rubien</t>
+  </si>
+  <si>
+    <t>Anke</t>
+  </si>
+  <si>
+    <t>DLRG Bz Kelsterbach e.V.</t>
+  </si>
+  <si>
+    <t>anke.rubien@gmx.de</t>
+  </si>
+  <si>
+    <t>Büttner</t>
+  </si>
+  <si>
+    <t>Jörg</t>
+  </si>
+  <si>
+    <t>mann-le@web.de</t>
+  </si>
+  <si>
+    <t>Schönberner</t>
+  </si>
+  <si>
+    <t>Polli</t>
+  </si>
+  <si>
+    <t>fashionschool4you@web.de</t>
+  </si>
+  <si>
+    <t>Stand 16.06.2023</t>
+  </si>
+  <si>
+    <t>400m</t>
+  </si>
+  <si>
+    <t>1000m</t>
+  </si>
+  <si>
+    <t>2500m</t>
   </si>
 </sst>
 </file>
@@ -651,7 +921,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,8 +953,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +972,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -775,6 +1059,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1090,26 +1386,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE04E44-FEC9-4434-BEAA-0C2D53DE9530}">
-  <dimension ref="A1:N201"/>
+  <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="183" zoomScaleNormal="100" zoomScaleSheetLayoutView="213" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.36328125" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" style="4"/>
+    <col min="12" max="13" width="11.54296875" style="4"/>
+    <col min="14" max="14" width="4" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>200</v>
+        <v>271</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1123,14 +1424,14 @@
       <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10">
-        <v>400</v>
-      </c>
-      <c r="G1" s="10">
-        <v>1000</v>
-      </c>
-      <c r="H1" s="10">
-        <v>2500</v>
+      <c r="F1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>290</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>4</v>
@@ -1147,29 +1448,42 @@
       <c r="M1" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="30">
+        <v>400</v>
+      </c>
+      <c r="O1" s="30">
+        <v>1000</v>
+      </c>
+      <c r="P1" s="30">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="F2" s="16">
         <f>SUM(F4:F201)</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G2" s="16">
         <f>SUM(G4:G201)</f>
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="H2" s="16">
         <f>SUM(H4:H201)</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="9">
         <f>SUM(L4:L201)</f>
-        <v>432</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>681</v>
+      </c>
+      <c r="M2" s="4">
+        <f>SUM(M4:M201)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1178,7 +1492,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1210,8 +1524,13 @@
         <f>IF(E4&gt;40908,(F4+G4+H4)*3,(F4+G4+H4)*6)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1246,8 +1565,15 @@
         <f t="shared" ref="L5:L68" si="0">IF(E5&gt;40908,(F5+G5+H5)*3,(F5+G5+H5)*6)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5" s="32"/>
+      <c r="O5" s="32">
+        <v>101</v>
+      </c>
+      <c r="P5" s="32">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1282,8 +1608,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6" s="32"/>
+      <c r="O6" s="32">
+        <v>102</v>
+      </c>
+      <c r="P6" s="32">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1318,8 +1651,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" s="32">
+        <v>1</v>
+      </c>
+      <c r="O7" s="32">
+        <v>103</v>
+      </c>
+      <c r="P7" s="32"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1354,8 +1694,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8" s="32">
+        <v>2</v>
+      </c>
+      <c r="O8" s="32">
+        <v>104</v>
+      </c>
+      <c r="P8" s="32"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1387,8 +1734,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1420,8 +1772,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1453,8 +1810,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11" s="32">
+        <v>3</v>
+      </c>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1486,8 +1848,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12" s="32">
+        <v>4</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1519,8 +1886,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1552,8 +1924,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14" s="32">
+        <v>5</v>
+      </c>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1585,8 +1962,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1618,8 +2000,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1651,8 +2038,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1684,8 +2076,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1717,8 +2114,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1750,8 +2152,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1789,8 +2196,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21" s="32">
+        <v>6</v>
+      </c>
+      <c r="O21" s="32">
+        <v>105</v>
+      </c>
+      <c r="P21" s="32">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1822,8 +2238,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1855,8 +2276,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
         <v>21</v>
       </c>
@@ -1890,9 +2316,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M24" s="21"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M24" s="25"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33">
+        <v>106</v>
+      </c>
+      <c r="P24" s="33"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1924,8 +2355,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N25" s="32"/>
+      <c r="O25" s="32">
+        <v>107</v>
+      </c>
+      <c r="P25" s="32"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
         <v>23</v>
       </c>
@@ -1959,9 +2395,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M26" s="21"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M26" s="25"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33">
+        <v>108</v>
+      </c>
+      <c r="P26" s="33"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1993,8 +2434,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2026,8 +2472,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2059,8 +2510,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2092,8 +2548,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30" s="32"/>
+      <c r="O30" s="32">
+        <v>109</v>
+      </c>
+      <c r="P30" s="32"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2125,8 +2586,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31" s="32">
+        <v>7</v>
+      </c>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2158,8 +2624,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N32" s="32"/>
+      <c r="O32" s="32">
+        <v>110</v>
+      </c>
+      <c r="P32" s="32"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2191,8 +2662,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2226,12 +2702,17 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2" t="s">
+      <c r="M34" s="5"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34">
+        <v>220</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2263,8 +2744,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N35" s="32">
+        <v>8</v>
+      </c>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2299,8 +2785,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N36" s="32">
+        <v>9</v>
+      </c>
+      <c r="O36" s="32">
+        <v>111</v>
+      </c>
+      <c r="P36" s="32"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2332,8 +2825,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N37" s="32"/>
+      <c r="O37" s="32">
+        <v>112</v>
+      </c>
+      <c r="P37" s="32"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2368,8 +2866,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N38" s="32"/>
+      <c r="O38" s="32">
+        <v>113</v>
+      </c>
+      <c r="P38" s="32">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2401,8 +2906,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2434,8 +2944,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N40" s="32"/>
+      <c r="O40" s="32">
+        <v>114</v>
+      </c>
+      <c r="P40" s="32"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2467,8 +2982,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N41" s="32"/>
+      <c r="O41" s="32">
+        <v>115</v>
+      </c>
+      <c r="P41" s="32"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2500,8 +3020,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N42" s="32">
+        <v>10</v>
+      </c>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2533,8 +3058,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2566,8 +3096,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N44" s="32">
+        <v>11</v>
+      </c>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2599,8 +3134,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N45" s="32">
+        <v>12</v>
+      </c>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2632,8 +3172,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N46" s="32">
+        <v>13</v>
+      </c>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2671,8 +3216,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N47" s="32">
+        <v>14</v>
+      </c>
+      <c r="O47" s="32">
+        <v>116</v>
+      </c>
+      <c r="P47" s="32">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>45</v>
       </c>
@@ -2704,8 +3258,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N48" s="32">
+        <v>15</v>
+      </c>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>46</v>
       </c>
@@ -2737,8 +3296,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>47</v>
       </c>
@@ -2770,8 +3334,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N50" s="32"/>
+      <c r="O50" s="32"/>
+      <c r="P50" s="32">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>48</v>
       </c>
@@ -2803,8 +3372,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N51" s="32">
+        <v>16</v>
+      </c>
+      <c r="O51" s="32"/>
+      <c r="P51" s="32"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>49</v>
       </c>
@@ -2836,8 +3410,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N52" s="32">
+        <v>17</v>
+      </c>
+      <c r="O52" s="32"/>
+      <c r="P52" s="32"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2869,8 +3448,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N53" s="32"/>
+      <c r="O53" s="32">
+        <v>117</v>
+      </c>
+      <c r="P53" s="32"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>51</v>
       </c>
@@ -2902,8 +3486,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N54" s="32"/>
+      <c r="O54" s="32">
+        <v>118</v>
+      </c>
+      <c r="P54" s="32"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>52</v>
       </c>
@@ -2935,8 +3524,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N55" s="32"/>
+      <c r="O55" s="32">
+        <v>119</v>
+      </c>
+      <c r="P55" s="32"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2965,8 +3559,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N56" s="32"/>
+      <c r="O56" s="32">
+        <v>120</v>
+      </c>
+      <c r="P56" s="32"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>54</v>
       </c>
@@ -2998,8 +3597,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N57" s="32">
+        <v>18</v>
+      </c>
+      <c r="O57" s="32">
+        <v>121</v>
+      </c>
+      <c r="P57" s="32"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>55</v>
       </c>
@@ -3028,8 +3634,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N58" s="32"/>
+      <c r="O58" s="32">
+        <v>122</v>
+      </c>
+      <c r="P58" s="32"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>56</v>
       </c>
@@ -3058,8 +3669,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N59" s="32"/>
+      <c r="O59" s="32">
+        <v>123</v>
+      </c>
+      <c r="P59" s="32"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>57</v>
       </c>
@@ -3091,8 +3707,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N60" s="32">
+        <v>19</v>
+      </c>
+      <c r="O60" s="32">
+        <v>124</v>
+      </c>
+      <c r="P60" s="32"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>58</v>
       </c>
@@ -3124,8 +3747,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N61" s="32">
+        <v>20</v>
+      </c>
+      <c r="O61" s="32">
+        <v>125</v>
+      </c>
+      <c r="P61" s="32"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>59</v>
       </c>
@@ -3157,8 +3787,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N62" s="32">
+        <v>21</v>
+      </c>
+      <c r="O62" s="32">
+        <v>126</v>
+      </c>
+      <c r="P62" s="32"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>60</v>
       </c>
@@ -3190,8 +3827,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N63" s="32">
+        <v>22</v>
+      </c>
+      <c r="O63" s="32">
+        <v>127</v>
+      </c>
+      <c r="P63" s="32"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>61</v>
       </c>
@@ -3223,8 +3867,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N64" s="32">
+        <v>23</v>
+      </c>
+      <c r="O64" s="32">
+        <v>128</v>
+      </c>
+      <c r="P64" s="32"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>62</v>
       </c>
@@ -3253,8 +3904,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N65" s="32"/>
+      <c r="O65" s="32">
+        <v>129</v>
+      </c>
+      <c r="P65" s="32"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>63</v>
       </c>
@@ -3283,8 +3939,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N66" s="32"/>
+      <c r="O66" s="32">
+        <v>130</v>
+      </c>
+      <c r="P66" s="32"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>64</v>
       </c>
@@ -3313,8 +3974,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N67" s="32"/>
+      <c r="O67" s="32">
+        <v>131</v>
+      </c>
+      <c r="P67" s="32"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>65</v>
       </c>
@@ -3346,8 +4012,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N68" s="32">
+        <v>24</v>
+      </c>
+      <c r="O68" s="32">
+        <v>132</v>
+      </c>
+      <c r="P68" s="32"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -3381,345 +4054,1423 @@
         <f t="shared" ref="L69:L132" si="1">IF(E69&gt;40908,(F69+G69+H69)*3,(F69+G69+H69)*6)</f>
         <v>6</v>
       </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2" t="s">
+      <c r="M69" s="5"/>
+      <c r="N69" s="34"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34">
+        <v>227</v>
+      </c>
+      <c r="Q69" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>67</v>
       </c>
+      <c r="B70" t="s">
+        <v>200</v>
+      </c>
+      <c r="C70" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="14">
+        <v>27376</v>
+      </c>
+      <c r="H70" s="11">
+        <v>1</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J70" t="s">
+        <v>11</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="L70" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N70" s="32"/>
+      <c r="O70" s="32"/>
+      <c r="P70" s="32">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>68</v>
       </c>
+      <c r="B71" t="s">
+        <v>200</v>
+      </c>
+      <c r="C71" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="14">
+        <v>39700</v>
+      </c>
+      <c r="F71" s="11">
+        <v>1</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" t="s">
+        <v>11</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="L71" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N71" s="32">
+        <v>25</v>
+      </c>
+      <c r="O71" s="32"/>
+      <c r="P71" s="32"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>69</v>
       </c>
+      <c r="B72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>204</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="14">
+        <v>40424</v>
+      </c>
+      <c r="F72" s="11">
+        <v>1</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J72" t="s">
+        <v>11</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="L72" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N72" s="32">
+        <v>26</v>
+      </c>
+      <c r="O72" s="32"/>
+      <c r="P72" s="32"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>70</v>
       </c>
+      <c r="B73" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="14">
+        <v>39724</v>
+      </c>
+      <c r="G73" s="11">
+        <v>1</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="J73" t="s">
+        <v>11</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="L73" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N73" s="32"/>
+      <c r="O73" s="32">
+        <v>133</v>
+      </c>
+      <c r="P73" s="32"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>71</v>
       </c>
+      <c r="B74" t="s">
+        <v>209</v>
+      </c>
+      <c r="C74" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="14">
+        <v>37519</v>
+      </c>
+      <c r="H74" s="11">
+        <v>1</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J74" t="s">
+        <v>210</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="L74" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A75">
+        <v>6</v>
+      </c>
+      <c r="N74" s="32"/>
+      <c r="O74" s="32"/>
+      <c r="P74" s="32">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="26">
         <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>212</v>
+      </c>
+      <c r="C75" t="s">
+        <v>213</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="14">
+        <v>39494</v>
+      </c>
+      <c r="G75" s="22">
+        <v>1</v>
+      </c>
+      <c r="H75" s="27">
+        <v>1</v>
+      </c>
+      <c r="I75" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J75" t="s">
+        <v>210</v>
+      </c>
+      <c r="K75" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="L75" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="N75" s="32"/>
+      <c r="O75" s="32">
+        <v>134</v>
+      </c>
+      <c r="P75" s="32">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>73</v>
       </c>
+      <c r="B76" t="s">
+        <v>214</v>
+      </c>
+      <c r="C76" t="s">
+        <v>215</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="14">
+        <v>38796</v>
+      </c>
+      <c r="H76" s="11">
+        <v>1</v>
+      </c>
+      <c r="I76" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J76" t="s">
+        <v>210</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="L76" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N76" s="32"/>
+      <c r="O76" s="32"/>
+      <c r="P76" s="32">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>74</v>
       </c>
+      <c r="B77" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77" t="s">
+        <v>217</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="14">
+        <v>38073</v>
+      </c>
+      <c r="G77" s="11">
+        <v>1</v>
+      </c>
+      <c r="I77" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J77" t="s">
+        <v>210</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="L77" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N77" s="32"/>
+      <c r="O77" s="32">
+        <v>135</v>
+      </c>
+      <c r="P77" s="32"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>75</v>
       </c>
+      <c r="B78" t="s">
+        <v>218</v>
+      </c>
+      <c r="C78" t="s">
+        <v>219</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="14">
+        <v>39422</v>
+      </c>
+      <c r="G78" s="11">
+        <v>1</v>
+      </c>
+      <c r="I78" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J78" t="s">
+        <v>210</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="L78" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N78" s="32"/>
+      <c r="O78" s="32">
+        <v>136</v>
+      </c>
+      <c r="P78" s="32"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>76</v>
       </c>
+      <c r="B79" t="s">
+        <v>220</v>
+      </c>
+      <c r="C79" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="14">
+        <v>41513</v>
+      </c>
+      <c r="F79" s="11">
+        <v>1</v>
+      </c>
+      <c r="I79" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="J79" t="s">
+        <v>11</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="L79" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="N79" s="32">
+        <v>27</v>
+      </c>
+      <c r="O79" s="32"/>
+      <c r="P79" s="32"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>77</v>
       </c>
+      <c r="B80" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="14">
+        <v>31950</v>
+      </c>
+      <c r="F80" s="11">
+        <v>1</v>
+      </c>
+      <c r="I80" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J80" t="s">
+        <v>11</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="L80" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N80" s="32">
+        <v>28</v>
+      </c>
+      <c r="O80" s="32"/>
+      <c r="P80" s="32"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>78</v>
       </c>
+      <c r="B81" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" t="s">
+        <v>227</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="14">
+        <v>40878</v>
+      </c>
+      <c r="F81" s="11">
+        <v>1</v>
+      </c>
+      <c r="G81" s="11">
+        <v>1</v>
+      </c>
+      <c r="I81" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J81" t="s">
+        <v>20</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="L81" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="N81" s="32">
+        <v>29</v>
+      </c>
+      <c r="O81" s="32">
+        <v>137</v>
+      </c>
+      <c r="P81" s="32"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>79</v>
       </c>
+      <c r="B82" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82" t="s">
+        <v>230</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" s="14">
+        <v>22123</v>
+      </c>
+      <c r="G82" s="11">
+        <v>1</v>
+      </c>
+      <c r="I82" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J82" t="s">
+        <v>231</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="L82" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N82" s="32"/>
+      <c r="O82" s="32">
+        <v>138</v>
+      </c>
+      <c r="P82" s="32"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>80</v>
       </c>
+      <c r="B83" t="s">
+        <v>233</v>
+      </c>
+      <c r="C83" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" s="14">
+        <v>40524</v>
+      </c>
+      <c r="G83" s="11">
+        <v>1</v>
+      </c>
+      <c r="I83" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J83" t="s">
+        <v>11</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="L83" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N83" s="32"/>
+      <c r="O83" s="32">
+        <v>139</v>
+      </c>
+      <c r="P83" s="32"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>81</v>
       </c>
+      <c r="B84" t="s">
+        <v>236</v>
+      </c>
+      <c r="C84" t="s">
+        <v>237</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="14">
+        <v>29450</v>
+      </c>
+      <c r="F84" s="11">
+        <v>1</v>
+      </c>
+      <c r="I84" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J84" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="L84" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N84" s="32">
+        <v>30</v>
+      </c>
+      <c r="O84" s="32"/>
+      <c r="P84" s="32"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>82</v>
       </c>
+      <c r="B85" t="s">
+        <v>236</v>
+      </c>
+      <c r="C85" t="s">
+        <v>239</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="14">
+        <v>40530</v>
+      </c>
+      <c r="F85" s="11">
+        <v>1</v>
+      </c>
+      <c r="I85" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J85" t="s">
+        <v>20</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="L85" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N85" s="32">
+        <v>31</v>
+      </c>
+      <c r="O85" s="32"/>
+      <c r="P85" s="32"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>83</v>
       </c>
+      <c r="B86" t="s">
+        <v>240</v>
+      </c>
+      <c r="C86" t="s">
+        <v>241</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" s="14">
+        <v>39355</v>
+      </c>
+      <c r="F86" s="11">
+        <v>1</v>
+      </c>
+      <c r="G86" s="11">
+        <v>1</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J86" t="s">
+        <v>242</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="L86" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="N86" s="32">
+        <v>32</v>
+      </c>
+      <c r="O86" s="32">
+        <v>140</v>
+      </c>
+      <c r="P86" s="32"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>84</v>
       </c>
+      <c r="B87" t="s">
+        <v>244</v>
+      </c>
+      <c r="C87" t="s">
+        <v>160</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="14">
+        <v>27214</v>
+      </c>
+      <c r="H87" s="11">
+        <v>1</v>
+      </c>
+      <c r="I87" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J87" t="s">
+        <v>20</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="L87" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N87" s="32"/>
+      <c r="O87" s="32"/>
+      <c r="P87" s="32">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>85</v>
       </c>
+      <c r="B88" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" t="s">
+        <v>247</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="14">
+        <v>22984</v>
+      </c>
+      <c r="H88" s="11">
+        <v>1</v>
+      </c>
+      <c r="I88" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J88" t="s">
+        <v>248</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="L88" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A89">
+        <v>6</v>
+      </c>
+      <c r="N88" s="32"/>
+      <c r="O88" s="32"/>
+      <c r="P88" s="32">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A89" s="2">
         <v>86</v>
       </c>
-      <c r="L89" s="4">
+      <c r="B89" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" s="15">
+        <v>40075</v>
+      </c>
+      <c r="F89" s="12">
+        <v>1</v>
+      </c>
+      <c r="G89" s="12">
+        <v>1</v>
+      </c>
+      <c r="H89" s="12"/>
+      <c r="I89" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K89" s="2"/>
+      <c r="L89" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="M89" s="5"/>
+      <c r="N89" s="34">
+        <v>33</v>
+      </c>
+      <c r="O89" s="34">
+        <v>141</v>
+      </c>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>87</v>
       </c>
+      <c r="B90" t="s">
+        <v>253</v>
+      </c>
+      <c r="C90" t="s">
+        <v>254</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="14">
+        <v>26655</v>
+      </c>
+      <c r="G90" s="11">
+        <v>1</v>
+      </c>
+      <c r="I90" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J90" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="L90" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N90" s="32"/>
+      <c r="O90" s="32">
+        <v>142</v>
+      </c>
+      <c r="P90" s="32"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>88</v>
       </c>
+      <c r="B91" t="s">
+        <v>256</v>
+      </c>
+      <c r="C91" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" s="14">
+        <v>41614</v>
+      </c>
+      <c r="F91" s="11">
+        <v>1</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J91" t="s">
+        <v>141</v>
+      </c>
       <c r="L91" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="N91" s="32">
+        <v>34</v>
+      </c>
+      <c r="O91" s="32"/>
+      <c r="P91" s="32"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>89</v>
       </c>
+      <c r="B92" t="s">
+        <v>257</v>
+      </c>
+      <c r="C92" t="s">
+        <v>258</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="14">
+        <v>38261</v>
+      </c>
+      <c r="G92" s="11">
+        <v>1</v>
+      </c>
+      <c r="I92" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J92" t="s">
+        <v>141</v>
+      </c>
       <c r="L92" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N92" s="32"/>
+      <c r="O92" s="32">
+        <v>143</v>
+      </c>
+      <c r="P92" s="32"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>90</v>
       </c>
+      <c r="B93" t="s">
+        <v>259</v>
+      </c>
+      <c r="C93" t="s">
+        <v>260</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="14">
+        <v>38523</v>
+      </c>
+      <c r="G93" s="11">
+        <v>1</v>
+      </c>
+      <c r="I93" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J93" t="s">
+        <v>141</v>
+      </c>
       <c r="L93" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N93" s="32"/>
+      <c r="O93" s="32">
+        <v>144</v>
+      </c>
+      <c r="P93" s="32"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>91</v>
       </c>
+      <c r="B94" t="s">
+        <v>261</v>
+      </c>
+      <c r="C94" t="s">
+        <v>262</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="14">
+        <v>40285</v>
+      </c>
+      <c r="F94" s="11">
+        <v>1</v>
+      </c>
+      <c r="I94" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J94" t="s">
+        <v>141</v>
+      </c>
       <c r="L94" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N94" s="32">
+        <v>35</v>
+      </c>
+      <c r="O94" s="32"/>
+      <c r="P94" s="32"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>92</v>
       </c>
+      <c r="B95" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="14">
+        <v>38918</v>
+      </c>
+      <c r="F95" s="11">
+        <v>1</v>
+      </c>
+      <c r="I95" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J95" t="s">
+        <v>141</v>
+      </c>
       <c r="L95" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N95" s="32">
+        <v>36</v>
+      </c>
+      <c r="O95" s="32"/>
+      <c r="P95" s="32"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>93</v>
       </c>
+      <c r="B96" t="s">
+        <v>263</v>
+      </c>
+      <c r="C96" t="s">
+        <v>264</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="14">
+        <v>38157</v>
+      </c>
+      <c r="G96" s="11">
+        <v>1</v>
+      </c>
+      <c r="I96" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J96" t="s">
+        <v>141</v>
+      </c>
       <c r="L96" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N96" s="32"/>
+      <c r="O96" s="32">
+        <v>145</v>
+      </c>
+      <c r="P96" s="32"/>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>94</v>
       </c>
+      <c r="B97" t="s">
+        <v>263</v>
+      </c>
+      <c r="C97" t="s">
+        <v>265</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="14">
+        <v>39352</v>
+      </c>
+      <c r="G97" s="11">
+        <v>1</v>
+      </c>
+      <c r="I97" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J97" t="s">
+        <v>141</v>
+      </c>
       <c r="L97" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N97" s="32"/>
+      <c r="O97" s="32">
+        <v>146</v>
+      </c>
+      <c r="P97" s="32"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>95</v>
       </c>
+      <c r="B98" t="s">
+        <v>266</v>
+      </c>
+      <c r="C98" t="s">
+        <v>65</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="14">
+        <v>42240</v>
+      </c>
+      <c r="F98" s="11">
+        <v>1</v>
+      </c>
+      <c r="I98" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J98" t="s">
+        <v>141</v>
+      </c>
       <c r="L98" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="N98" s="32">
+        <v>37</v>
+      </c>
+      <c r="O98" s="32"/>
+      <c r="P98" s="32"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>96</v>
       </c>
+      <c r="B99" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" t="s">
+        <v>268</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="14">
+        <v>38870</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1</v>
+      </c>
+      <c r="I99" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J99" t="s">
+        <v>141</v>
+      </c>
       <c r="L99" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N99" s="32"/>
+      <c r="O99" s="32">
+        <v>147</v>
+      </c>
+      <c r="P99" s="32"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>97</v>
       </c>
+      <c r="B100" t="s">
+        <v>263</v>
+      </c>
+      <c r="C100" t="s">
+        <v>269</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="14">
+        <v>28142</v>
+      </c>
+      <c r="F100" s="11">
+        <v>1</v>
+      </c>
+      <c r="I100" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J100" t="s">
+        <v>141</v>
+      </c>
       <c r="L100" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N100" s="32">
+        <v>38</v>
+      </c>
+      <c r="O100" s="32"/>
+      <c r="P100" s="32"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>98</v>
       </c>
+      <c r="B101" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" t="s">
+        <v>270</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="14">
+        <v>27050</v>
+      </c>
+      <c r="F101" s="11">
+        <v>1</v>
+      </c>
+      <c r="I101" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J101" t="s">
+        <v>141</v>
+      </c>
       <c r="L101" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="N101" s="32">
+        <v>39</v>
+      </c>
+      <c r="O101" s="32"/>
+      <c r="P101" s="32"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>99</v>
       </c>
+      <c r="B102" t="s">
+        <v>272</v>
+      </c>
+      <c r="C102" t="s">
+        <v>273</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" s="14">
+        <v>26063</v>
+      </c>
+      <c r="F102" s="11">
+        <v>1</v>
+      </c>
+      <c r="G102" s="11">
+        <v>1</v>
+      </c>
+      <c r="H102" s="11">
+        <v>1</v>
+      </c>
+      <c r="I102" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J102" t="s">
+        <v>20</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="L102" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="N102" s="29">
+        <v>40</v>
+      </c>
+      <c r="O102" s="29">
+        <v>148</v>
+      </c>
+      <c r="P102" s="29">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>100</v>
       </c>
+      <c r="B103" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
+        <v>275</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" s="14">
+        <v>26385</v>
+      </c>
+      <c r="H103" s="11">
+        <v>1</v>
+      </c>
+      <c r="I103" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J103" t="s">
+        <v>20</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="L103" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="P103" s="29">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>101</v>
       </c>
+      <c r="B104" t="s">
+        <v>277</v>
+      </c>
+      <c r="C104" t="s">
+        <v>278</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="14">
+        <v>23072</v>
+      </c>
+      <c r="H104" s="11">
+        <v>1</v>
+      </c>
+      <c r="I104" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J104" t="s">
+        <v>279</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="L104" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="P104" s="29">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>102</v>
       </c>
+      <c r="B105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C105" t="s">
+        <v>282</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="14">
+        <v>24530</v>
+      </c>
+      <c r="H105" s="11">
+        <v>1</v>
+      </c>
+      <c r="I105" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" t="s">
+        <v>20</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="L105" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A106">
+        <v>6</v>
+      </c>
+      <c r="P105" s="29">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A106" s="2">
         <v>103</v>
       </c>
-      <c r="L106" s="4">
+      <c r="B106" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="15">
+        <v>39339</v>
+      </c>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12">
+        <v>1</v>
+      </c>
+      <c r="H106" s="12"/>
+      <c r="I106" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K106" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="L106" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="M106" s="5"/>
+      <c r="N106" s="31"/>
+      <c r="O106" s="31">
+        <v>149</v>
+      </c>
+      <c r="P106" s="31"/>
+      <c r="Q106" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>104</v>
       </c>
@@ -3728,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>105</v>
       </c>
@@ -3737,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>106</v>
       </c>
@@ -3746,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>107</v>
       </c>
@@ -3755,7 +5506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>108</v>
       </c>
@@ -3764,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>109</v>
       </c>
@@ -4534,7 +6285,7 @@
         <v>194</v>
       </c>
       <c r="L197" s="4">
-        <f t="shared" ref="L197:L201" si="3">IF(E197&gt;40908,(F197+G197+H197)*3,(F197+G197+H197)*6)</f>
+        <f>IF(E197&gt;40908,(F197+G197+H197)*3,(F197+G197+H197)*6)</f>
         <v>0</v>
       </c>
     </row>
@@ -4543,7 +6294,7 @@
         <v>195</v>
       </c>
       <c r="L198" s="4">
-        <f t="shared" si="3"/>
+        <f>IF(E198&gt;40908,(F198+G198+H198)*3,(F198+G198+H198)*6)</f>
         <v>0</v>
       </c>
     </row>
@@ -4552,7 +6303,7 @@
         <v>196</v>
       </c>
       <c r="L199" s="4">
-        <f t="shared" si="3"/>
+        <f>IF(E199&gt;40908,(F199+G199+H199)*3,(F199+G199+H199)*6)</f>
         <v>0</v>
       </c>
     </row>
@@ -4561,18 +6312,18 @@
         <v>197</v>
       </c>
       <c r="L200" s="4">
-        <f t="shared" si="3"/>
+        <f>IF(E200&gt;40908,(F200+G200+H200)*3,(F200+G200+H200)*6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="L201" s="4">
-        <f t="shared" si="3"/>
+        <f>IF(E201&gt;40908,(F201+G201+H201)*3,(F201+G201+H201)*6)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:M2" xr:uid="{2EE04E44-FEC9-4434-BEAA-0C2D53DE9530}"/>
+  <autoFilter ref="A3:M201" xr:uid="{2EE04E44-FEC9-4434-BEAA-0C2D53DE9530}"/>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" xr:uid="{39F95526-6589-48D9-9256-2C3A96BC98CB}"/>
     <hyperlink ref="K5" r:id="rId2" xr:uid="{4B13F389-BE3A-4D2E-8EBD-C446DED172A1}"/>
@@ -4591,7 +6342,36 @@
     <hyperlink ref="K53" r:id="rId15" xr:uid="{7EF9AED8-12FE-42EB-A0F4-33F8B10B1AA5}"/>
     <hyperlink ref="K54" r:id="rId16" xr:uid="{E6C3C767-9D2E-4FBE-937E-344A000814A1}"/>
     <hyperlink ref="K55" r:id="rId17" xr:uid="{32D9A79A-B069-4D5B-A6BD-23B46C904CFF}"/>
+    <hyperlink ref="K70" r:id="rId18" xr:uid="{A24D671E-0865-4451-A366-B1D781E4DF68}"/>
+    <hyperlink ref="K71" r:id="rId19" xr:uid="{164EEB79-5F99-4C84-8BB4-6DF1DD995B83}"/>
+    <hyperlink ref="K72" r:id="rId20" xr:uid="{1B85CB8E-D11E-4B28-8EFB-68230CC05E8C}"/>
+    <hyperlink ref="K73" r:id="rId21" xr:uid="{571AC509-65CE-47AC-A596-D1FB0EE19F26}"/>
+    <hyperlink ref="K74" r:id="rId22" xr:uid="{59827D3C-47DB-4B86-A1B3-F65483726FA3}"/>
+    <hyperlink ref="K75" r:id="rId23" xr:uid="{4162BD41-37D8-4331-BC22-C20BC5B645A3}"/>
+    <hyperlink ref="K76" r:id="rId24" xr:uid="{99966627-E0D4-49C0-A243-148426D98615}"/>
+    <hyperlink ref="K77" r:id="rId25" xr:uid="{514337D2-AC7A-4744-B173-AFD0EDAA35DD}"/>
+    <hyperlink ref="K78" r:id="rId26" xr:uid="{E002CB01-5DB5-474F-81BC-8D4DAD2EAD75}"/>
+    <hyperlink ref="K79" r:id="rId27" xr:uid="{827CE4E4-C833-4DB1-980D-47D100B261B9}"/>
+    <hyperlink ref="K80" r:id="rId28" xr:uid="{DAEEB19E-231F-4736-BF56-31380CBCF258}"/>
+    <hyperlink ref="K81" r:id="rId29" xr:uid="{F14E9C52-FAC5-419C-AC7D-966E1E849A47}"/>
+    <hyperlink ref="K82" r:id="rId30" xr:uid="{3D5EE0DF-CF6E-4178-931B-F1D89CF67C1B}"/>
+    <hyperlink ref="K83" r:id="rId31" xr:uid="{D97B2C72-A989-49C3-B029-5D3FD44E631A}"/>
+    <hyperlink ref="K84" r:id="rId32" xr:uid="{6CF231DA-2B8F-4ACB-A7F5-2ABE8C5EE85A}"/>
+    <hyperlink ref="K85" r:id="rId33" xr:uid="{94411CC4-ED70-45EA-8419-2743004AE41F}"/>
+    <hyperlink ref="K86" r:id="rId34" xr:uid="{F238DFFC-2500-43BF-879A-0420BEF21A10}"/>
+    <hyperlink ref="K87" r:id="rId35" xr:uid="{69220783-0D60-45B5-8355-2D14CAB355F4}"/>
+    <hyperlink ref="K88" r:id="rId36" xr:uid="{B62C6078-C5B3-4B1C-BA89-893048731AB9}"/>
+    <hyperlink ref="K90" r:id="rId37" xr:uid="{94E59C27-9E0B-4AC8-9EE8-3BC25E74AE6C}"/>
+    <hyperlink ref="K102" r:id="rId38" xr:uid="{AFE02828-3265-4603-A7BC-1D887E6ADAF0}"/>
+    <hyperlink ref="K103" r:id="rId39" xr:uid="{F4747A96-46AC-4769-BE4B-1A9DD7C4B33F}"/>
+    <hyperlink ref="K104" r:id="rId40" xr:uid="{48476D0A-F98C-43C4-8617-91E325B242C4}"/>
+    <hyperlink ref="K105" r:id="rId41" xr:uid="{02F718BF-5D3E-4E32-AB98-47E1F034C25A}"/>
+    <hyperlink ref="K106" r:id="rId42" xr:uid="{2A502EFD-78B6-493F-A921-0E8BE7BC2827}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId43"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="16" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>